<commit_message>
fixing straing in hbrown 090320
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_09.03.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_09.03.20.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">90minuteinduction</t>
   </si>
   <si>
-    <t xml:space="preserve">TYD451</t>
+    <t xml:space="preserve">TDY1441</t>
   </si>
   <si>
     <t xml:space="preserve">CNAG_03894</t>
@@ -303,14 +303,15 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,7 +343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
corrected strain and CNAG#
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_09.03.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_09.03.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BE37F1-16FF-C24C-8036-5A5F159860E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03B462C-DA00-354E-9580-D25E89E874BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="460" windowWidth="23060" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4080" windowWidth="23060" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="59">
   <si>
     <t>harvestDate</t>
   </si>
@@ -60,13 +60,7 @@
     <t>90minuteinduction</t>
   </si>
   <si>
-    <t>CNAG_00000</t>
-  </si>
-  <si>
     <t>DMEM.37C.CO2</t>
-  </si>
-  <si>
-    <t>TDY451</t>
   </si>
   <si>
     <t>TDY1325</t>
@@ -562,7 +556,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,7 +599,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -617,13 +611,13 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2">
         <v>90</v>
@@ -634,25 +628,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3">
         <v>90</v>
@@ -663,7 +657,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -675,13 +669,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <v>90</v>
@@ -692,7 +686,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -704,13 +698,13 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5">
         <v>90</v>
@@ -721,7 +715,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -733,13 +727,13 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6">
         <v>90</v>
@@ -750,7 +744,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -762,13 +756,13 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7">
         <v>90</v>
@@ -779,7 +773,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -791,13 +785,13 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8">
         <v>90</v>
@@ -808,7 +802,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -820,13 +814,13 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9">
         <v>90</v>
@@ -837,7 +831,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -849,13 +843,13 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10">
         <v>90</v>
@@ -866,7 +860,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -878,13 +872,13 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11">
         <v>90</v>
@@ -895,7 +889,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -907,13 +901,13 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12">
         <v>90</v>
@@ -924,7 +918,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -936,13 +930,13 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H13">
         <v>90</v>
@@ -953,7 +947,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -965,13 +959,13 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14">
         <v>90</v>
@@ -982,7 +976,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -994,13 +988,13 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15">
         <v>90</v>
@@ -1011,7 +1005,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -1023,13 +1017,13 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16">
         <v>90</v>
@@ -1040,7 +1034,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -1052,13 +1046,13 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17">
         <v>90</v>
@@ -1069,7 +1063,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -1081,13 +1075,13 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H18">
         <v>90</v>
@@ -1098,7 +1092,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -1110,13 +1104,13 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19">
         <v>90</v>
@@ -1127,7 +1121,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -1139,13 +1133,13 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20">
         <v>90</v>
@@ -1156,7 +1150,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -1168,13 +1162,13 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21">
         <v>90</v>
@@ -1185,7 +1179,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -1197,13 +1191,13 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H22">
         <v>90</v>
@@ -1214,7 +1208,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -1226,13 +1220,13 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H23">
         <v>90</v>
@@ -1243,7 +1237,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -1255,13 +1249,13 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H24">
         <v>90</v>
@@ -1272,7 +1266,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1284,13 +1278,13 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25">
         <v>90</v>

</xml_diff>